<commit_message>
Testing fineshed. Found a minor incongruence with the paper results
</commit_message>
<xml_diff>
--- a/comparison_results.xlsx
+++ b/comparison_results.xlsx
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>35099.98</v>
+        <v>78507.97</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>30323.47</v>
+        <v>31460.08</v>
       </c>
     </row>
     <row r="4">
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>23886.33</v>
+        <v>27657.51</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>79721.46000000001</v>
+        <v>116789.4</v>
       </c>
     </row>
     <row r="6">
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>25502.09</v>
+        <v>71157.02</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>4868.63</v>
+        <v>12877.46</v>
       </c>
     </row>
     <row r="9">
@@ -609,7 +609,7 @@
         <v>-0</v>
       </c>
       <c r="E9" t="n">
-        <v>24282.58</v>
+        <v>79904.2</v>
       </c>
     </row>
     <row r="10">
@@ -628,7 +628,7 @@
         <v>-0</v>
       </c>
       <c r="E10" t="n">
-        <v>7195.36</v>
+        <v>13325.17</v>
       </c>
     </row>
     <row r="11">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>12811.06</v>
+        <v>70035.75999999999</v>
       </c>
     </row>
     <row r="12">
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>25991.12</v>
+        <v>27127.73</v>
       </c>
     </row>
     <row r="14">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>5674.32</v>
+        <v>6620.4</v>
       </c>
     </row>
     <row r="15">
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>10042.47</v>
+        <v>13025.25</v>
       </c>
     </row>
     <row r="17">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>567.05</v>
+        <v>2248.97</v>
       </c>
     </row>
     <row r="18">
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>8319.219999999999</v>
+        <v>21695.74</v>
       </c>
     </row>
     <row r="19">
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>3536.33</v>
+        <v>4035.65</v>
       </c>
     </row>
     <row r="20">
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1457.98</v>
+        <v>1957.3</v>
       </c>
     </row>
     <row r="21">
@@ -837,7 +837,7 @@
         <v>-0</v>
       </c>
       <c r="E21" t="n">
-        <v>5937.68</v>
+        <v>16817.6</v>
       </c>
     </row>
     <row r="22">
@@ -856,7 +856,7 @@
         <v>-0</v>
       </c>
       <c r="E22" t="n">
-        <v>10600.88</v>
+        <v>19904</v>
       </c>
     </row>
     <row r="23">
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>12206.37</v>
+        <v>14026.26</v>
       </c>
     </row>
     <row r="24">
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>6039.83</v>
+        <v>12130.22</v>
       </c>
     </row>
     <row r="25">
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>4236.02</v>
+        <v>4847.03</v>
       </c>
     </row>
     <row r="26">
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>15154.71</v>
+        <v>16521.27</v>
       </c>
     </row>
     <row r="27">
@@ -951,7 +951,7 @@
         <v>-0</v>
       </c>
       <c r="E27" t="n">
-        <v>4855.92</v>
+        <v>5328.96</v>
       </c>
     </row>
     <row r="28">
@@ -1008,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>3832.79</v>
+        <v>5343.89</v>
       </c>
     </row>
     <row r="31">
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>4436.89</v>
+        <v>5047.9</v>
       </c>
     </row>
     <row r="32">
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>5533.57</v>
+        <v>9225.91</v>
       </c>
     </row>
     <row r="33">
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>8899.92</v>
+        <v>10831.5</v>
       </c>
     </row>
     <row r="35">

</xml_diff>